<commit_message>
Layout atualizado e icone da loja
</commit_message>
<xml_diff>
--- a/Info/Games_Names.xlsx
+++ b/Info/Games_Names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ander\Documents\GitHub\PlayStoreProject\Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F97FD9-9381-4E7E-BAE4-DD20F0E4E9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1AB6FF-2297-4CCF-AB6E-C37F2EE0E47F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6CBC7CB4-3457-4BEB-A3AA-981853889B9A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="187" xr2:uid="{6CBC7CB4-3457-4BEB-A3AA-981853889B9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="88">
   <si>
     <t>Nome</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Caves</t>
   </si>
   <si>
-    <t>Variações</t>
-  </si>
-  <si>
     <t>Todo dia</t>
   </si>
   <si>
@@ -64,247 +61,241 @@
     <t>Varia</t>
   </si>
   <si>
-    <t>Blocão?</t>
-  </si>
-  <si>
     <t>Sim</t>
   </si>
   <si>
-    <t>Fácil</t>
-  </si>
-  <si>
-    <t>Médio</t>
-  </si>
-  <si>
     <t>Não</t>
   </si>
   <si>
-    <t>https://www.addictinggames.com/funny/skydrop</t>
-  </si>
-  <si>
-    <t>Dragon Hunter</t>
-  </si>
-  <si>
     <t>Facil</t>
   </si>
   <si>
-    <t>https://www.addictinggames.com/action/dragon-hunter</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/clicker/fast-circles</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/puzzle/match-the-animal</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/action/speed-billiards</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/clicker/knifemaster</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/clicker/sticky-balls</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/action/bottle-flip-challenge</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/clicker/tower-rush</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/clicker/neon-block</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/action/snakes-and-circles</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/puzzle/kids-zoo-fun</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/shooting/stack-colors</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/action/passage</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/puzzle/can-you-do-it</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/action/triangle-way</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/action/badminton-brawl</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/puzzle/ring-fall</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/action/soldiers-fury</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/action/block-dodger</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/action/colored-downhill</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/clicker/beat-hop</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/action/gemotrical-dash</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/clicker/balls-and-bricks</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/shooting/spiral-paint</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/puzzle/boxing-punches</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/action/jack-o-copter</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/shooting/knife-rain</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/clicker/tower-breaker</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/action/parapals</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/action/jump-monkey</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/puzzle/look-look</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/puzzle/put-bacon</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/puzzle/jelly-jumper</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/clicker/juice-bottle</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/clicker/jump-bottle</t>
-  </si>
-  <si>
-    <t>https://www.addictinggames.com/clicker/flappybird-classic</t>
-  </si>
-  <si>
-    <t>Fast Circles</t>
-  </si>
-  <si>
-    <t>Match-The Animal</t>
-  </si>
-  <si>
-    <t>Speed Billiards</t>
-  </si>
-  <si>
-    <t>Knifemaster Knifemaster</t>
-  </si>
-  <si>
     <t>Sticky Balls</t>
   </si>
   <si>
-    <t>Bottle-Flip Challenge</t>
-  </si>
-  <si>
-    <t>Tower Rush</t>
-  </si>
-  <si>
-    <t>Neon Block</t>
-  </si>
-  <si>
-    <t>Snakes-And Circles</t>
-  </si>
-  <si>
-    <t>Kids-Zoo Fun</t>
-  </si>
-  <si>
-    <t>Stack Colors</t>
-  </si>
-  <si>
-    <t>Passage Passage</t>
-  </si>
-  <si>
-    <t>Can-You-Do It</t>
-  </si>
-  <si>
-    <t>Triangle Way</t>
-  </si>
-  <si>
-    <t>Badminton Brawl</t>
-  </si>
-  <si>
-    <t>Ring Fall</t>
-  </si>
-  <si>
-    <t>Soldiers Fury</t>
-  </si>
-  <si>
-    <t>Block Dodger</t>
-  </si>
-  <si>
-    <t>Colored Downhill</t>
-  </si>
-  <si>
-    <t>Beat Hop</t>
-  </si>
-  <si>
-    <t>Gemotrical Dash</t>
-  </si>
-  <si>
-    <t>Balls-And Bricks</t>
-  </si>
-  <si>
-    <t>Spiral Paint</t>
-  </si>
-  <si>
-    <t>Boxing Punches</t>
-  </si>
-  <si>
-    <t>Jack-O Copter</t>
-  </si>
-  <si>
-    <t>Knife Rain</t>
-  </si>
-  <si>
-    <t>Tower Breaker</t>
-  </si>
-  <si>
-    <t>Parapals Parapals</t>
-  </si>
-  <si>
-    <t>Jump Monkey</t>
-  </si>
-  <si>
-    <t>Look Look</t>
-  </si>
-  <si>
-    <t>Put Bacon</t>
-  </si>
-  <si>
-    <t>Jelly Jumper</t>
-  </si>
-  <si>
-    <t>Juice Bottle</t>
-  </si>
-  <si>
-    <t>Jump Bottle</t>
-  </si>
-  <si>
-    <t>Flappybird Classic</t>
-  </si>
-  <si>
-    <t>Difícil</t>
-  </si>
-  <si>
     <t>Dificil</t>
+  </si>
+  <si>
+    <t>Variacoes</t>
+  </si>
+  <si>
+    <t>Blocao</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24925</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24937</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24950</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24948</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24899</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24907</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24961</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24788</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24729</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24714</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/23614</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24705</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24699</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24694</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24685</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24686</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24682</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24680</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24677</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24919</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24656</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24647</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24650</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24642</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24644</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/23716</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24621</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/23651</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24626</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24587</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24592</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/23594</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/23914</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/23565</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/23571</t>
+  </si>
+  <si>
+    <t>https://www.addictinggames.com/embed/html5-games/24032</t>
+  </si>
+  <si>
+    <t>DragonHunter</t>
+  </si>
+  <si>
+    <t>FastCircles</t>
+  </si>
+  <si>
+    <t>MatchTheAnimal</t>
+  </si>
+  <si>
+    <t>SpeedBilliards</t>
+  </si>
+  <si>
+    <t>Knifemaster</t>
+  </si>
+  <si>
+    <t>BottleFlipChallenge</t>
+  </si>
+  <si>
+    <t>TowerRush</t>
+  </si>
+  <si>
+    <t>NeonBlock</t>
+  </si>
+  <si>
+    <t>SnakesAndCircles</t>
+  </si>
+  <si>
+    <t>KidsZooFun</t>
+  </si>
+  <si>
+    <t>StackColors</t>
+  </si>
+  <si>
+    <t>PassagePassage</t>
+  </si>
+  <si>
+    <t>CanYouDoIt</t>
+  </si>
+  <si>
+    <t>TriangleWay</t>
+  </si>
+  <si>
+    <t>BadmintonBrawl</t>
+  </si>
+  <si>
+    <t>RingFall</t>
+  </si>
+  <si>
+    <t>SoldiersFury</t>
+  </si>
+  <si>
+    <t>BlockDodger</t>
+  </si>
+  <si>
+    <t>ColoredDownhill</t>
+  </si>
+  <si>
+    <t>BeatHop</t>
+  </si>
+  <si>
+    <t>GemotricalDash</t>
+  </si>
+  <si>
+    <t>BallsAndBricks</t>
+  </si>
+  <si>
+    <t>SpiralPaint</t>
+  </si>
+  <si>
+    <t>BoxingPunches</t>
+  </si>
+  <si>
+    <t>JackOCopter</t>
+  </si>
+  <si>
+    <t>KnifeRain</t>
+  </si>
+  <si>
+    <t>TowerBreaker</t>
+  </si>
+  <si>
+    <t>ParapalsParapals</t>
+  </si>
+  <si>
+    <t>JumpMonkey</t>
+  </si>
+  <si>
+    <t>PutBacon</t>
+  </si>
+  <si>
+    <t>JellyJumper</t>
+  </si>
+  <si>
+    <t>JuiceBottle</t>
+  </si>
+  <si>
+    <t>JumpBottle</t>
+  </si>
+  <si>
+    <t>FlappybirdClassic</t>
+  </si>
+  <si>
+    <t>Medio</t>
+  </si>
+  <si>
+    <t>Nao</t>
   </si>
 </sst>
 </file>
@@ -674,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AA9F81-F3A9-49DE-B83A-02AA0B078B37}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,7 +676,7 @@
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="121.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -693,16 +684,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -713,759 +704,739 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="D2" s="1">
         <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1">
         <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>87</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1">
         <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>87</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>89</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1">
         <v>7</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1">
         <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>87</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="1">
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="D8" s="1">
         <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1">
         <v>9</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="D10" s="1">
         <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="D11" s="1">
         <v>10</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1">
         <v>6</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>26</v>
+        <v>87</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="D13" s="1">
         <v>8</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>27</v>
+        <v>9</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" s="1">
         <v>5</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>28</v>
+        <v>87</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="D15" s="1">
         <v>6</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D16" s="1">
         <v>9</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>30</v>
+        <v>9</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D17" s="1">
         <v>8</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D18" s="1">
         <v>8</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D19" s="1">
         <v>10</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>33</v>
+        <v>9</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D20" s="1">
         <v>8</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>90</v>
+        <v>13</v>
       </c>
       <c r="D21" s="1">
         <v>7</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>35</v>
+        <v>87</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>89</v>
+        <v>13</v>
       </c>
       <c r="D22" s="1">
         <v>7</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>36</v>
+        <v>9</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>90</v>
+        <v>13</v>
       </c>
       <c r="D23" s="1">
         <v>6</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="D24" s="1">
         <v>8</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>90</v>
+        <v>13</v>
       </c>
       <c r="D25" s="1">
         <v>8</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="D26" s="1">
         <v>8</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D27" s="1">
         <v>8</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="D28" s="1">
         <v>9</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>42</v>
+        <v>9</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>89</v>
+        <v>13</v>
       </c>
       <c r="D29" s="1">
         <v>7</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="D30" s="1">
         <v>6</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="D31" s="1">
         <v>7</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>45</v>
+        <v>87</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D32" s="1">
         <v>5</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D33" s="1">
         <v>7</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="D34" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>48</v>
+        <v>9</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="D35" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D36" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="D37" s="1">
         <v>8</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="D38" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D39" s="1">
-        <v>9</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1486,27 +1457,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{B81C40C5-DBC7-4707-BE32-67ABC94FBF21}"/>
-    <hyperlink ref="F17" r:id="rId2" xr:uid="{97E0D2F6-43CB-48AC-A2F5-77F7104629F4}"/>
-    <hyperlink ref="F18" r:id="rId3" xr:uid="{F4173E2E-23E0-4F25-B638-25E6236EC4C5}"/>
-    <hyperlink ref="F20" r:id="rId4" xr:uid="{DA53D5AC-8925-4D31-92AA-AD0ED4ACC58B}"/>
-    <hyperlink ref="F23" r:id="rId5" xr:uid="{B5912B9C-EE3C-4584-8064-42A338E468E9}"/>
-    <hyperlink ref="F24" r:id="rId6" xr:uid="{D4E6402E-BF5D-4A12-A54E-4AFBE18700D0}"/>
-    <hyperlink ref="F25" r:id="rId7" xr:uid="{877E4912-3DD5-4A7C-AC85-E2D84EF54F97}"/>
-    <hyperlink ref="F26" r:id="rId8" xr:uid="{F3B0AECB-80B0-4726-B2E3-ED233DE4FEA7}"/>
-    <hyperlink ref="F27" r:id="rId9" xr:uid="{CC69389D-9A13-49AD-9F45-1F235FC9E2BA}"/>
-    <hyperlink ref="F29" r:id="rId10" xr:uid="{95C5D7D2-35EB-4D84-94A5-91EB6A66118A}"/>
-    <hyperlink ref="F30" r:id="rId11" xr:uid="{96BC9172-D917-4BB8-A448-1C16AB0190C9}"/>
-    <hyperlink ref="F32" r:id="rId12" xr:uid="{52E3F852-5AAB-43CD-B7A6-BC2AEEE91C13}"/>
-    <hyperlink ref="F33" r:id="rId13" xr:uid="{3173F62C-5F7E-405C-8FAE-1721268FC596}"/>
-    <hyperlink ref="F35" r:id="rId14" xr:uid="{CB29DDB9-13F3-4038-96F0-0D04632545EC}"/>
-    <hyperlink ref="F36" r:id="rId15" xr:uid="{A8C260AF-8DA1-4FD6-8DFE-0207450797AD}"/>
-    <hyperlink ref="F37" r:id="rId16" xr:uid="{3E269CBA-8A67-4A8E-9BFF-7D574025C54A}"/>
-    <hyperlink ref="F38" r:id="rId17" xr:uid="{2D2300A6-18B7-4106-BE20-26159ACD2EC6}"/>
-    <hyperlink ref="F39" r:id="rId18" xr:uid="{1DA3EAE2-F80E-4092-A7C0-D4FE08499D94}"/>
-    <hyperlink ref="F10" r:id="rId19" xr:uid="{FF73AE44-52C6-4E9D-B7AD-6A964AC102D0}"/>
-    <hyperlink ref="F15" r:id="rId20" xr:uid="{AABF0F49-9891-417E-A4AC-3AB8DA318009}"/>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{CB218000-C033-497C-B055-443D024B791D}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{0C7AA982-8A91-4E97-9345-2F3192173A1D}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{1CE5EBFE-D7D6-474D-8D40-6C6D33C9D4C7}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{65F32AB9-F798-4F1E-A823-16DE8A91DB6E}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{D03D961E-25EF-40A9-A881-5595623222AC}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{E7E6A64C-EC4A-4E84-AAAB-6C8059780ACF}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{7D7B5140-61DD-43BD-A34B-71695270F2B0}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{424F2247-61DF-4485-9022-6ED38F25D520}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{8687E634-E1A4-4CE0-84A7-57E37B41B5A9}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{60D402BB-771B-4E0E-9696-20286A4DD300}"/>
+    <hyperlink ref="F12" r:id="rId11" xr:uid="{6548F164-0493-4265-9806-83B035C8FF1C}"/>
+    <hyperlink ref="F13" r:id="rId12" xr:uid="{FC2FA328-BF76-4077-9AE5-92D79F85C8BB}"/>
+    <hyperlink ref="F14" r:id="rId13" xr:uid="{405D8109-262C-4B42-BE09-F9E56ACAE72F}"/>
+    <hyperlink ref="F15" r:id="rId14" xr:uid="{AD831896-BF83-4F9D-B315-0BD1E9E02782}"/>
+    <hyperlink ref="F16" r:id="rId15" xr:uid="{004DB047-92FD-43D9-A4DF-D60AC9F67E1A}"/>
+    <hyperlink ref="F17" r:id="rId16" xr:uid="{23D10AC8-0EAB-44FA-9437-4B5E0F2360CA}"/>
+    <hyperlink ref="F18" r:id="rId17" xr:uid="{FC6AC05C-CC16-4017-B42C-D0D11E62C7F4}"/>
+    <hyperlink ref="F19" r:id="rId18" xr:uid="{63CE1249-78CE-4740-8A77-7047957A1DA5}"/>
+    <hyperlink ref="F20" r:id="rId19" xr:uid="{FB2E6A11-F52C-41B2-BBAB-EDC7B02B728F}"/>
+    <hyperlink ref="F21" r:id="rId20" xr:uid="{A4F7A27B-DAA4-4820-8698-4F5FDAE082FD}"/>
+    <hyperlink ref="F22" r:id="rId21" xr:uid="{A706B141-B2F2-429E-A14C-5453E3ED0806}"/>
+    <hyperlink ref="F23" r:id="rId22" xr:uid="{49A29ABB-83E2-479B-92C7-D228676F57B6}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>